<commit_message>
build: add XLSX files for testing
</commit_message>
<xml_diff>
--- a/resources/files/example.sheet-hidden.xlsx
+++ b/resources/files/example.sheet-hidden.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7380" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7380"/>
   </bookViews>
   <sheets>
     <sheet name="Cell Object" sheetId="1" r:id="rId1"/>
     <sheet name="Parsing Options" sheetId="2" r:id="rId2"/>
-    <sheet name="HIDDEN" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="HIDDEN" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -546,11 +546,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="54.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -650,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -825,10 +828,15 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>